<commit_message>
Add unit to 2022 demand column
</commit_message>
<xml_diff>
--- a/code/h2_demand_refineries.xlsx
+++ b/code/h2_demand_refineries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Library/CloudStorage/OneDrive-IdahoNationalLaboratory/Documents/Research/Hydrogen from Nuclear/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A876BDAB-F779-9646-A811-A50A64F4618E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CBC6E1-B3A8-4727-8CDB-6326339EDC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="18200" windowHeight="8500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>refinery_id</t>
   </si>
   <si>
-    <t>demand_2022</t>
-  </si>
-  <si>
     <t>iso</t>
   </si>
   <si>
@@ -411,6 +408,9 @@
   </si>
   <si>
     <t>SINCLAIR WYOMING REFINING CO</t>
+  </si>
+  <si>
+    <t>demand_2022 (kg/day)</t>
   </si>
 </sst>
 </file>
@@ -880,16 +880,16 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="9.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="19" width="9.1328125" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="32" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -948,15 +948,15 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="D2" s="11">
         <v>6</v>
@@ -1007,12 +1007,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -1066,12 +1066,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -1125,12 +1125,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -1180,12 +1180,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -1239,12 +1239,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>
@@ -1298,12 +1298,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
@@ -1357,12 +1357,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1416,12 +1416,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>14</v>
@@ -1475,12 +1475,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -1506,12 +1506,12 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>16</v>
@@ -1566,12 +1566,12 @@
       </c>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
@@ -1625,12 +1625,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1682,12 +1682,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -1741,12 +1741,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>22</v>
@@ -1800,12 +1800,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
@@ -1859,12 +1859,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>24</v>
@@ -1918,12 +1918,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>25</v>
@@ -1975,12 +1975,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
@@ -2014,12 +2014,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>8</v>
@@ -2073,12 +2073,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>28</v>
@@ -2132,12 +2132,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>29</v>
@@ -2191,12 +2191,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>30</v>
@@ -2250,12 +2250,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>31</v>
@@ -2299,12 +2299,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2358,12 +2358,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>33</v>
@@ -2417,12 +2417,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>34</v>
@@ -2476,12 +2476,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>35</v>
@@ -2535,12 +2535,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>36</v>
@@ -2594,12 +2594,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>38</v>
@@ -2653,12 +2653,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>39</v>
@@ -2712,12 +2712,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>39</v>
@@ -2771,12 +2771,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>40</v>
@@ -2830,12 +2830,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>41</v>
@@ -2889,12 +2889,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>42</v>
@@ -2946,12 +2946,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>43</v>
@@ -3005,12 +3005,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>44</v>
@@ -3064,12 +3064,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>45</v>
@@ -3107,12 +3107,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>46</v>
@@ -3142,12 +3142,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>47</v>
@@ -3189,12 +3189,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>48</v>
@@ -3248,12 +3248,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>50</v>
@@ -3301,12 +3301,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>51</v>
@@ -3356,12 +3356,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>52</v>
@@ -3415,12 +3415,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>53</v>
@@ -3474,12 +3474,12 @@
         <v>186</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>54</v>
@@ -3531,12 +3531,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>55</v>
@@ -3590,16 +3590,16 @@
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="14"/>
     </row>
-    <row r="50" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
     </row>
-    <row r="51" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
       <c r="D51" s="15"/>
@@ -3626,17 +3626,17 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3650,13 +3650,13 @@
         <v>57</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="str">
         <f>original!A2</f>
         <v>ALABAMA</v>
@@ -3682,7 +3682,7 @@
         <v>Southeast</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="str">
         <f>original!A3</f>
         <v>ALASKA</v>
@@ -3708,7 +3708,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="str">
         <f>original!A4</f>
         <v>ARKANSAS</v>
@@ -3734,7 +3734,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="str">
         <f>original!A5</f>
         <v>ARKANSAS</v>
@@ -3760,7 +3760,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="str">
         <f>original!A6</f>
         <v>CALIFORNIA</v>
@@ -3786,7 +3786,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="str">
         <f>original!A7</f>
         <v>CALIFORNIA</v>
@@ -3812,7 +3812,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="str">
         <f>original!A8</f>
         <v>CALIFORNIA</v>
@@ -3838,7 +3838,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="str">
         <f>original!A9</f>
         <v>CALIFORNIA</v>
@@ -3864,7 +3864,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="str">
         <f>original!A10</f>
         <v>CALIFORNIA</v>
@@ -3890,7 +3890,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="str">
         <f>original!A11</f>
         <v>CALIFORNIA</v>
@@ -3916,7 +3916,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="str">
         <f>original!A12</f>
         <v>CALIFORNIA</v>
@@ -3942,7 +3942,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="str">
         <f>original!A13</f>
         <v>CALIFORNIA</v>
@@ -3968,7 +3968,7 @@
         <v>CAISO</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="str">
         <f>original!A14</f>
         <v>COLORADO</v>
@@ -3994,7 +3994,7 @@
         <v>Southwest</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="str">
         <f>original!A15</f>
         <v>DELAWARE</v>
@@ -4020,7 +4020,7 @@
         <v>PJM</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="str">
         <f>original!A16</f>
         <v>HAWAII</v>
@@ -4046,7 +4046,7 @@
         <v>None</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="str">
         <f>original!A17</f>
         <v>ILLINOIS</v>
@@ -4072,7 +4072,7 @@
         <v>PJM</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="str">
         <f>original!A18</f>
         <v>ILLINOIS</v>
@@ -4098,7 +4098,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="str">
         <f>original!A19</f>
         <v>KANSAS</v>
@@ -4124,7 +4124,7 @@
         <v>SPP</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="str">
         <f>original!A20</f>
         <v>KANSAS</v>
@@ -4150,7 +4150,7 @@
         <v>SPP</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="str">
         <f>original!A21</f>
         <v>KANSAS</v>
@@ -4176,7 +4176,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="str">
         <f>original!A22</f>
         <v>LOUISIANA</v>
@@ -4202,7 +4202,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="str">
         <f>original!A23</f>
         <v>LOUISIANA</v>
@@ -4228,7 +4228,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="str">
         <f>original!A24</f>
         <v>LOUISIANA</v>
@@ -4254,7 +4254,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="str">
         <f>original!A25</f>
         <v>LOUISIANA</v>
@@ -4280,7 +4280,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="str">
         <f>original!A26</f>
         <v>MINNESOTA</v>
@@ -4306,7 +4306,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="str">
         <f>original!A27</f>
         <v>MINNESOTA</v>
@@ -4332,7 +4332,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="str">
         <f>original!A28</f>
         <v>MISSISSIPPI</v>
@@ -4358,7 +4358,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="str">
         <f>original!A29</f>
         <v>MISSISSIPPI</v>
@@ -4384,7 +4384,7 @@
         <v>MISO</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="str">
         <f>original!A30</f>
         <v>MONTANA</v>
@@ -4410,7 +4410,7 @@
         <v>Northwest</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="str">
         <f>original!A31</f>
         <v>MONTANA</v>
@@ -4436,7 +4436,7 @@
         <v>Northwest</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="str">
         <f>original!A32</f>
         <v>MONTANA</v>
@@ -4462,7 +4462,7 @@
         <v>Northwest</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="str">
         <f>original!A33</f>
         <v>MONTANA</v>
@@ -4488,7 +4488,7 @@
         <v>Northwest</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="str">
         <f>original!A34</f>
         <v>NEW JERSEY</v>
@@ -4514,7 +4514,7 @@
         <v>PJM</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="str">
         <f>original!A35</f>
         <v>NEW JERSEY</v>
@@ -4540,7 +4540,7 @@
         <v>PJM</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="str">
         <f>original!A36</f>
         <v>NEW MEXICO</v>
@@ -4566,7 +4566,7 @@
         <v>Southwest</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="str">
         <f>original!A37</f>
         <v>OKLAHOMA</v>
@@ -4592,7 +4592,7 @@
         <v>SPP</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="str">
         <f>original!A38</f>
         <v>OKLAHOMA</v>
@@ -4618,7 +4618,7 @@
         <v>SPP</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="str">
         <f>original!A39</f>
         <v>OKLAHOMA</v>
@@ -4644,7 +4644,7 @@
         <v>SPP</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="str">
         <f>original!A40</f>
         <v>PENNSYLVANIA</v>
@@ -4670,7 +4670,7 @@
         <v>PJM</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="str">
         <f>original!A41</f>
         <v>TENNESSEE</v>
@@ -4696,7 +4696,7 @@
         <v>Southeast</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="str">
         <f>original!A42</f>
         <v>TEXAS</v>
@@ -4722,7 +4722,7 @@
         <v>ERCOT</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="str">
         <f>original!A43</f>
         <v>TEXAS</v>
@@ -4748,7 +4748,7 @@
         <v>SPP</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="str">
         <f>original!A44</f>
         <v>TEXAS</v>
@@ -4774,7 +4774,7 @@
         <v>Southwest</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="str">
         <f>original!A45</f>
         <v>TEXAS</v>
@@ -4800,7 +4800,7 @@
         <v>SPP</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="str">
         <f>original!A46</f>
         <v>WASHINGTON</v>
@@ -4826,7 +4826,7 @@
         <v>Northwest</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="str">
         <f>original!A47</f>
         <v>WEST VIRGINIA</v>
@@ -4852,7 +4852,7 @@
         <v>PJM</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="str">
         <f>original!A48</f>
         <v>WYOMING</v>
@@ -4878,37 +4878,37 @@
         <v>Northwest</v>
       </c>
     </row>
-    <row r="49" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="50" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="51" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="52" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="53" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="54" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="55" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="56" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="57" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="58" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="59" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="60" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="61" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="62" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="63" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="64" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="70" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="71" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="72" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
     </row>
-    <row r="74" spans="1:5" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" s="7" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B74" s="18"/>
       <c r="C74" s="18"/>
       <c r="E74" s="8"/>
@@ -4931,13 +4931,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B2,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>ALABAMA</v>
@@ -4962,7 +4962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B3,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>ALASKA</v>
@@ -4974,7 +4974,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B4,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>ARKANSAS</v>
@@ -4986,7 +4986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B5,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>ARKANSAS</v>
@@ -4998,7 +4998,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B6,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5010,7 +5010,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B7,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5022,7 +5022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B8,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5034,7 +5034,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B9,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5046,7 +5046,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B10,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5058,7 +5058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B11,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5070,7 +5070,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B12,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5082,7 +5082,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B13,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>CALIFORNIA</v>
@@ -5094,7 +5094,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B14,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>COLORADO</v>
@@ -5106,7 +5106,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B15,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>DELAWARE</v>
@@ -5118,7 +5118,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B16,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>HAWAII</v>
@@ -5130,7 +5130,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B17,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>ILLINOIS</v>
@@ -5142,7 +5142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B18,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>ILLINOIS</v>
@@ -5154,7 +5154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B19,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>KANSAS</v>
@@ -5166,7 +5166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B20,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>KANSAS</v>
@@ -5178,7 +5178,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B21,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>LOUISIANA</v>
@@ -5190,7 +5190,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B22,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>LOUISIANA</v>
@@ -5202,7 +5202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B23,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>LOUISIANA</v>
@@ -5214,7 +5214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B24,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>LOUISIANA</v>
@@ -5226,7 +5226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B25,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>MINNESOTA</v>
@@ -5238,7 +5238,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B26,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>MINNESOTA</v>
@@ -5250,7 +5250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B27,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>MISSISSIPPI</v>
@@ -5262,7 +5262,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B28,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>MISSISSIPPI</v>
@@ -5274,7 +5274,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B29,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>MONTANA</v>
@@ -5286,7 +5286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B30,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>MONTANA</v>
@@ -5298,7 +5298,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B31,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>MONTANA</v>
@@ -5310,7 +5310,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B32,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>NEW JERSEY</v>
@@ -5322,7 +5322,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B33,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>NEW JERSEY</v>
@@ -5334,7 +5334,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B34,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>NEW MEXICO</v>
@@ -5346,7 +5346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B35,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>OKLAHOMA</v>
@@ -5358,7 +5358,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B36,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>OKLAHOMA</v>
@@ -5370,7 +5370,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B37,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>OKLAHOMA</v>
@@ -5382,7 +5382,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B38,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>PENNSYLVANIA</v>
@@ -5394,7 +5394,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B39,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>TENNESSEE</v>
@@ -5406,7 +5406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B40,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>TEXAS</v>
@@ -5418,7 +5418,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B41,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>TEXAS</v>
@@ -5430,7 +5430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B42,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>TEXAS</v>
@@ -5442,7 +5442,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B43,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>TEXAS</v>
@@ -5454,7 +5454,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B44,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>WASHINGTON</v>
@@ -5466,7 +5466,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B45,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>WEST VIRGINIA</v>
@@ -5478,7 +5478,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="str">
         <f>_xlfn.XLOOKUP(Iso_state_map!B46,processed!C$2:C$48,processed!A$2:A$48)</f>
         <v>WYOMING</v>

</xml_diff>

<commit_message>
Compute annual carbon emissions
</commit_message>
<xml_diff>
--- a/code/h2_demand_refineries.xlsx
+++ b/code/h2_demand_refineries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CBC6E1-B3A8-4727-8CDB-6326339EDC17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782B3003-1869-435D-8E99-A3E2F3F0DAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3623,7 +3623,7 @@
   <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>